<commit_message>
Testing of valid user registration
</commit_message>
<xml_diff>
--- a/src/main/java/org/zalando/frontend/qa/testdata/testdata.xlsx
+++ b/src/main/java/org/zalando/frontend/qa/testdata/testdata.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\eclipse-workspaceSelenium\AutomationFrameworkE2E\src\main\java\org\zalando\frontend\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD35892-7118-4B70-9A2E-86B310EABD91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AA8367-75BC-4B1A-B7EA-58FB657C35CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C430A504-51EA-4D72-8A04-E0046A4CF670}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C430A504-51EA-4D72-8A04-E0046A4CF670}"/>
   </bookViews>
   <sheets>
     <sheet name="newsletter" sheetId="1" r:id="rId1"/>
+    <sheet name="registration" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Email Address</t>
   </si>
@@ -58,6 +60,45 @@
   </si>
   <si>
     <t>testmailzalando123@gmail.com</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Washi</t>
+  </si>
+  <si>
+    <t>Sundar</t>
+  </si>
+  <si>
+    <t>hikip</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>testmail</t>
+  </si>
+  <si>
+    <t>zalando</t>
+  </si>
+  <si>
+    <t>zalandopwdpuma</t>
   </si>
 </sst>
 </file>
@@ -444,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE8FE5-AD77-488E-9D41-78541CC6E2B4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,4 +545,142 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87B5307-2F30-4BD5-8522-EC9DC45775B0}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{66FAD177-697A-4375-A0DD-730A23E5486C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D47E442-5556-4683-A610-CCC50645123C}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{0B8B5479-DE8C-40D4-BA56-F8406D707830}"/>
+    <hyperlink ref="D2" r:id="rId2" display="fashionzalandotest123@gmail.com" xr:uid="{9A30ED0E-7FF0-49B5-BFC0-3FCE91689216}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{36133A9B-0465-4A1A-90BD-708BDDF83B59}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>